<commit_message>
EPBDS-9046 Add more tests
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9046_Vocabulary_comparison.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9046_Vocabulary_comparison.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpushko/openl-tablets/STUDIO/org.openl.rules.test/test-resources/functionality/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA1304F9-477E-D142-8B25-D747DC77C499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="22035" windowHeight="10545"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="18280" windowHeight="15400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t xml:space="preserve">Datatype MyColor &lt;String&gt; </t>
   </si>
@@ -66,29 +72,169 @@
     <t>Step2</t>
   </si>
   <si>
-    <t>validateComparisonLiteralWithDomainTypeInternal(b1, b2, method, node, bindingContext);</t>
+    <t>Step3</t>
+  </si>
+  <si>
+    <t>= someColor&lt;&gt;"Pink"?0:1</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>Step5</t>
+  </si>
+  <si>
+    <t>Step6</t>
+  </si>
+  <si>
+    <t>= someColor!=" "?0:1</t>
+  </si>
+  <si>
+    <t>= someColor&lt;&gt;""?0:1</t>
+  </si>
+  <si>
+    <t>Step7</t>
+  </si>
+  <si>
+    <t>Step8</t>
+  </si>
+  <si>
+    <t>Step9</t>
+  </si>
+  <si>
+    <t>= someColor=="yellow"?0:1</t>
+  </si>
+  <si>
+    <t>= someColor!="yellow"?0:1</t>
+  </si>
+  <si>
+    <t>= someColor&lt;&gt;"yellow"?0:1</t>
+  </si>
+  <si>
+    <t>//Validate warning message for vocabulary value comparison</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult mySpr1(MyObject someObject)</t>
+  </si>
+  <si>
+    <t>= someColor=="Yellow"?0:1</t>
+  </si>
+  <si>
+    <t>= someColor!="Yellow"?0:1</t>
+  </si>
+  <si>
+    <t>= someColor=="."?0:1</t>
+  </si>
+  <si>
+    <t>//Validate warning message for vocabulary value comparison in a SimpleRules Table</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>boolean conditionParam</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>=someColor == "Pink"</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>MyObject someObject</t>
+  </si>
+  <si>
+    <t>some object</t>
+  </si>
+  <si>
+    <t>String conditionParam</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>=someColor != "Pink"</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>boolean res</t>
+  </si>
+  <si>
+    <t>someColor == "Pink"</t>
+  </si>
+  <si>
+    <t>Rules boolean MyRules1(MyObject someObject)</t>
+  </si>
+  <si>
+    <t>SmartRules Double MyRules2(MyObject someObject)</t>
+  </si>
+  <si>
+    <t>Conditions One</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some object </t>
+  </si>
+  <si>
+    <t>Returns One</t>
+  </si>
+  <si>
+    <t>Condition1</t>
+  </si>
+  <si>
+    <t>(someColor == "Pink")?res</t>
+  </si>
+  <si>
+    <t>//Validate warning message for vocabulary value comparison in a SmartRules Table and External Tables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCF086"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,11 +247,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,14 +285,22 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFFCF086"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -191,7 +349,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +382,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,6 +434,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,19 +626,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="2" max="2" width="32.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -454,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -465,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -476,17 +668,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -494,7 +686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -502,13 +694,34 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -516,24 +729,295 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="44.83203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="40.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.5" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>